<commit_message>
3 row in 1 line demo.
</commit_message>
<xml_diff>
--- a/BPM组件需求整理.xlsx
+++ b/BPM组件需求整理.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25220" windowHeight="9660" activeTab="1"/>
+    <workbookView windowWidth="25600" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="母版" sheetId="4" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123">
   <si>
     <t>大分类</t>
   </si>
@@ -285,9 +285,6 @@
     <t>v-textfield支持字数限制、报错、placeholder、后缀功能</t>
   </si>
   <si>
-    <t>只读需要使用disabled属性，可能需要自实现</t>
-  </si>
-  <si>
     <t>规则校验需要自实现</t>
   </si>
   <si>
@@ -413,9 +410,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
@@ -428,7 +425,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -450,23 +447,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -479,8 +474,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -489,52 +485,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -550,7 +500,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -564,15 +536,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -618,12 +615,96 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -636,169 +717,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -867,15 +864,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -886,6 +874,56 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -907,36 +945,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -950,99 +958,88 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="28" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1051,7 +1048,7 @@
     <xf numFmtId="42" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1060,56 +1057,56 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1132,9 +1129,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1889,10 +1883,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1917,7 +1911,7 @@
       <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
+      <c r="E1" s="11" t="s">
         <v>81</v>
       </c>
     </row>
@@ -1934,24 +1928,30 @@
       <c r="D2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="3" ht="17" spans="1:5">
       <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="14" t="s">
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="11" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="4" ht="17" spans="1:5">
       <c r="A4" s="6"/>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
+      <c r="B4" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="E4" s="12" t="s">
         <v>84</v>
       </c>
@@ -1959,513 +1959,501 @@
     <row r="5" ht="17" spans="1:5">
       <c r="A5" s="6"/>
       <c r="B5" s="8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="6" ht="17" spans="1:5">
       <c r="A6" s="6"/>
       <c r="B6" s="8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="11" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="7" ht="17" spans="1:5">
       <c r="A7" s="6"/>
       <c r="B7" s="8" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="13" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="8" ht="17" spans="1:5">
       <c r="A8" s="6"/>
       <c r="B8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="E8" s="14" t="s">
-        <v>88</v>
+        <v>20</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="13" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="9" ht="17" spans="1:5">
       <c r="A9" s="6"/>
       <c r="B9" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="14" t="s">
-        <v>86</v>
+      <c r="D9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="10" ht="17" spans="1:5">
       <c r="A10" s="6"/>
       <c r="B10" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="8"/>
+        <v>23</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>24</v>
+      </c>
       <c r="D10" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="14" t="s">
-        <v>86</v>
+        <v>25</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="11" ht="17" spans="1:5">
       <c r="A11" s="6"/>
       <c r="B11" s="8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="13" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="12" ht="17" spans="1:5">
       <c r="A12" s="6"/>
       <c r="B12" s="8" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="13" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="13" ht="17" spans="1:5">
       <c r="A13" s="6"/>
-      <c r="B13" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="E13" s="14" t="s">
+      <c r="B13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="13" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="14" ht="17" spans="1:5">
       <c r="A14" s="6"/>
-      <c r="B14" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="E14" s="14" t="s">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="13" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="15" ht="17" spans="1:5">
       <c r="A15" s="6"/>
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="14" t="s">
-        <v>93</v>
+      <c r="B15" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="16" ht="17" spans="1:5">
       <c r="A16" s="6"/>
       <c r="B16" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="8"/>
+        <v>36</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="D16" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="E16" s="13" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="17" ht="17" spans="1:5">
       <c r="A17" s="6"/>
-      <c r="B17" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C17" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="E17" s="14" t="s">
+      <c r="B17" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="18" ht="17" spans="1:5">
       <c r="A18" s="6"/>
-      <c r="B18" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="E18" s="12" t="s">
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="11" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="19" ht="17" spans="1:5">
       <c r="A19" s="6"/>
-      <c r="B19" s="8"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="12" t="s">
+      <c r="B19" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E19" s="11" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="20" ht="17" spans="1:5">
       <c r="A20" s="6"/>
       <c r="B20" s="8" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="E20" s="13" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="21" ht="17" spans="1:5">
       <c r="A21" s="6"/>
       <c r="B21" s="8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D21" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="11" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="22" ht="17" spans="1:5">
-      <c r="A22" s="6"/>
+      <c r="A22" s="7"/>
       <c r="B22" s="8" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="E22" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="13" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="23" ht="17" spans="1:5">
-      <c r="A23" s="7"/>
+      <c r="A23" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="B23" s="8" t="s">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="8"/>
-      <c r="E23" s="14" t="s">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="13" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="24" ht="17" spans="1:5">
-      <c r="A24" s="5" t="s">
-        <v>52</v>
-      </c>
+      <c r="A24" s="6"/>
       <c r="B24" s="8" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>102</v>
+        <v>22</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E24" s="12" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="25" ht="17" spans="1:5">
       <c r="A25" s="6"/>
-      <c r="B25" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>54</v>
+      <c r="B25" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="E25" s="13" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" ht="17" spans="1:5">
       <c r="A26" s="6"/>
-      <c r="B26" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E26" s="14" t="s">
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="11" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="27" ht="17" spans="1:5">
       <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="B27" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>108</v>
+      </c>
       <c r="E27" s="12" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="28" ht="34" spans="1:5">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="28" ht="17" spans="1:5">
       <c r="A28" s="6"/>
-      <c r="B28" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E28" s="13" t="s">
+      <c r="B28" s="6"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="12" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="29" ht="17" spans="1:5">
       <c r="A29" s="6"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="6"/>
-      <c r="D29" s="6"/>
+      <c r="B29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="E29" s="13" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="30" ht="17" spans="1:5">
       <c r="A30" s="6"/>
-      <c r="B30" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="E30" s="14" t="s">
+      <c r="B30" s="6"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="11" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="31" ht="17" spans="1:5">
       <c r="A31" s="6"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
+      <c r="B31" s="6"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
       <c r="E31" s="12" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="32" ht="17" spans="1:5">
-      <c r="A32" s="6"/>
-      <c r="B32" s="10"/>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="13" t="s">
+      <c r="A32" s="7"/>
+      <c r="B32" s="7"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="7"/>
+      <c r="E32" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="33" ht="17" spans="1:5">
-      <c r="A33" s="7"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="13" t="s">
+    <row r="33" ht="34" spans="1:5">
+      <c r="A33" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="34" ht="17" spans="1:5">
+      <c r="A34" s="6"/>
+      <c r="B34" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="E34" s="11" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="34" ht="34" spans="1:5">
-      <c r="A34" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>67</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="35" ht="17" spans="1:5">
       <c r="A35" s="6"/>
       <c r="B35" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C35" s="8"/>
+        <v>71</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>72</v>
+      </c>
       <c r="D35" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="E35" s="12" t="s">
-        <v>116</v>
+        <v>73</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="36" ht="17" spans="1:5">
       <c r="A36" s="6"/>
       <c r="B36" s="8" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C36" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>73</v>
-      </c>
+        <v>75</v>
+      </c>
+      <c r="D36" s="8"/>
       <c r="E36" s="12" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" ht="17" spans="1:5">
       <c r="A37" s="6"/>
       <c r="B37" s="8" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="C37" s="8" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" s="8"/>
-      <c r="E37" s="13" t="s">
-        <v>86</v>
+        <v>77</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="38" ht="17" spans="1:5">
       <c r="A38" s="6"/>
-      <c r="B38" s="8" t="s">
-        <v>76</v>
-      </c>
-      <c r="C38" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="E38" s="12" t="s">
+      <c r="B38" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E38" s="11" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="39" ht="17" spans="1:5">
       <c r="A39" s="6"/>
-      <c r="B39" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D39" s="9" t="s">
-        <v>80</v>
-      </c>
-      <c r="E39" s="12" t="s">
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="13" t="s">
         <v>118</v>
       </c>
     </row>
     <row r="40" ht="17" spans="1:5">
-      <c r="A40" s="6"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="10"/>
-      <c r="E40" s="14" t="s">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7"/>
+      <c r="E40" s="12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="41" ht="17" spans="1:5">
-      <c r="A41" s="7"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="11"/>
-      <c r="D41" s="11"/>
-      <c r="E41" s="13" t="s">
-        <v>120</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="A2:A23"/>
-    <mergeCell ref="A24:A33"/>
-    <mergeCell ref="A34:A41"/>
-    <mergeCell ref="B2:B4"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B33"/>
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="C2:C4"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="C30:C33"/>
-    <mergeCell ref="C39:C41"/>
-    <mergeCell ref="D2:D4"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="D30:D33"/>
-    <mergeCell ref="D39:D41"/>
+  <mergeCells count="24">
+    <mergeCell ref="A2:A22"/>
+    <mergeCell ref="A23:A32"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C32"/>
+    <mergeCell ref="C38:C40"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="D25:D26"/>
+    <mergeCell ref="D27:D28"/>
+    <mergeCell ref="D29:D32"/>
+    <mergeCell ref="D38:D40"/>
   </mergeCells>
   <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -2496,13 +2484,13 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:5">

</xml_diff>